<commit_message>
Added new entries to Watchlist
</commit_message>
<xml_diff>
--- a/Watchlist.xlsx
+++ b/Watchlist.xlsx
@@ -16,7 +16,7 @@
     <sheet name="Port" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$B$1:$B$501</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$B$1:$B$500</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="413">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="466" uniqueCount="423">
   <si>
     <t>Name</t>
   </si>
@@ -405,12 +405,6 @@
     <t>ULTA</t>
   </si>
   <si>
-    <t>DSW</t>
-  </si>
-  <si>
-    <t>10 times 2017 P/E</t>
-  </si>
-  <si>
     <t>ORCL</t>
   </si>
   <si>
@@ -1270,6 +1264,42 @@
   </si>
   <si>
     <t>330M net income, 300 shares out standing</t>
+  </si>
+  <si>
+    <t>Roku</t>
+  </si>
+  <si>
+    <t>ROKU</t>
+  </si>
+  <si>
+    <t>100M Shares, this year Sales about 700M,future unknown,</t>
+  </si>
+  <si>
+    <t>5.27/share this year, own about 35% of its land</t>
+  </si>
+  <si>
+    <t>2.85/share excluding land sales,estimating $700M land sales,309M diluted shares</t>
+  </si>
+  <si>
+    <t>GreenSky</t>
+  </si>
+  <si>
+    <t>GSKY</t>
+  </si>
+  <si>
+    <t>400M estimated sales this year, 190M shares, 100M net income this year</t>
+  </si>
+  <si>
+    <t>Perspecta</t>
+  </si>
+  <si>
+    <t>PRSP</t>
+  </si>
+  <si>
+    <t>1.8-1.95/share EPS this year,8-12% EPS growth next 3 years, 3-5% Rev growth,peers trade at around 18</t>
+  </si>
+  <si>
+    <t>290M shares, 7.9/share next twelve months</t>
   </si>
 </sst>
 </file>
@@ -1634,10 +1664,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:N501"/>
+  <dimension ref="A1:N500"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A75" workbookViewId="0">
-      <selection activeCell="I106" sqref="I106"/>
+    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="F50" sqref="F50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1657,33 +1687,33 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D1" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="E1" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="F1" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="G1" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="B2" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="C2">
         <v>22.55</v>
@@ -1700,7 +1730,7 @@
         <v>0</v>
       </c>
       <c r="G2" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="H2" s="2">
         <v>1.1662084257206207</v>
@@ -1711,10 +1741,10 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="B3" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="C3">
         <v>11.55</v>
@@ -1731,7 +1761,7 @@
         <v>0</v>
       </c>
       <c r="G3" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="H3" s="2">
         <v>0.76965891251605179</v>
@@ -1742,10 +1772,10 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B4" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="C4">
         <v>29.1</v>
@@ -1761,7 +1791,7 @@
         <v>3</v>
       </c>
       <c r="G4" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="H4" s="2">
         <v>0.75257731958762875</v>
@@ -1793,7 +1823,7 @@
         <v>9.1891891891891895</v>
       </c>
       <c r="G5" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="H5" s="2">
         <v>0.74534094936656492</v>
@@ -1804,7 +1834,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B6" t="s">
         <v>5</v>
@@ -1824,7 +1854,7 @@
         <v>0</v>
       </c>
       <c r="G6" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="H6" s="2">
         <v>0.66116184184962112</v>
@@ -1855,7 +1885,7 @@
         <v>1</v>
       </c>
       <c r="G7" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="H7" s="2">
         <v>0.63696369636963701</v>
@@ -1866,10 +1896,10 @@
     </row>
     <row r="8" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C8" s="3">
         <v>281.74</v>
@@ -1887,7 +1917,7 @@
         <v>41.478129713423833</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="H8" s="4">
         <v>0.55853824129539276</v>
@@ -1918,7 +1948,7 @@
         <v>0</v>
       </c>
       <c r="G9" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="H9" s="2">
         <v>0.54053533602927017</v>
@@ -1929,10 +1959,10 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="B10" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="C10">
         <v>19.55</v>
@@ -1950,7 +1980,7 @@
         <v>4.7619047619047619</v>
       </c>
       <c r="G10" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="H10" s="2">
         <v>0.53939836804286945</v>
@@ -1961,10 +1991,10 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="B11" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C11">
         <v>35.25</v>
@@ -1981,7 +2011,7 @@
         <v>0</v>
       </c>
       <c r="G11" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="H11" s="2">
         <v>0.48936170212765956</v>
@@ -2021,10 +2051,10 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="B14" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C14">
         <v>172.44</v>
@@ -2041,7 +2071,7 @@
         <v>30</v>
       </c>
       <c r="G14" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="I14" s="2">
         <v>0.5</v>
@@ -2049,10 +2079,10 @@
     </row>
     <row r="15" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C15" s="3">
         <v>223.63</v>
@@ -2070,7 +2100,7 @@
         <v>8.146639511201629</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="H15" s="4"/>
       <c r="I15" s="4">
@@ -2079,10 +2109,10 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="B16" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="C16">
         <v>65.67</v>
@@ -2090,10 +2120,10 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B17" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C17">
         <v>130.94</v>
@@ -2121,7 +2151,7 @@
         <v>0</v>
       </c>
       <c r="G18" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="I18" s="2">
         <v>0.6</v>
@@ -2129,10 +2159,10 @@
     </row>
     <row r="19" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="C19" s="3">
         <v>257.02</v>
@@ -2174,7 +2204,7 @@
         <v>2.8037383177570092</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="H21" s="4"/>
       <c r="I21" s="4">
@@ -2183,10 +2213,10 @@
     </row>
     <row r="22" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="C22" s="3">
         <v>1427.05</v>
@@ -2196,7 +2226,7 @@
     </row>
     <row r="23" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>103</v>
@@ -2209,10 +2239,10 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="B24" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C24">
         <v>13.33</v>
@@ -2222,10 +2252,10 @@
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B25" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C25">
         <v>157.01</v>
@@ -2233,10 +2263,10 @@
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="B26" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="C26">
         <v>85.4</v>
@@ -2255,10 +2285,10 @@
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B28" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C28">
         <v>65.849999999999994</v>
@@ -2275,7 +2305,7 @@
         <v>0</v>
       </c>
       <c r="G28" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="I28" s="2">
         <v>0.5</v>
@@ -2283,10 +2313,10 @@
     </row>
     <row r="29" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C29" s="3">
         <v>175.36</v>
@@ -2304,7 +2334,7 @@
         <v>14.6</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="H29" s="4"/>
       <c r="I29" s="4">
@@ -2313,10 +2343,10 @@
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="B30" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="C30">
         <v>29.9</v>
@@ -2327,7 +2357,7 @@
         <v>89</v>
       </c>
       <c r="B31" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="C31">
         <v>22.25</v>
@@ -2359,10 +2389,10 @@
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B34" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C34">
         <v>82.26</v>
@@ -2370,10 +2400,10 @@
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="B35" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="C35">
         <v>29.7</v>
@@ -2381,10 +2411,10 @@
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="B36" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="C36">
         <v>177.21</v>
@@ -2392,10 +2422,10 @@
     </row>
     <row r="37" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B37" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C37">
         <v>119.16</v>
@@ -2425,10 +2455,10 @@
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="B40" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="C40">
         <v>17.47</v>
@@ -2445,7 +2475,7 @@
         <v>0</v>
       </c>
       <c r="G40" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="I40" s="2">
         <v>0.65</v>
@@ -2453,16 +2483,16 @@
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B41" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C41">
         <v>17.059999999999999</v>
       </c>
       <c r="G41" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="42" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -2487,7 +2517,7 @@
         <v>0</v>
       </c>
       <c r="G42" s="3" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="H42" s="4"/>
       <c r="I42" s="4">
@@ -2496,10 +2526,10 @@
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B43" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="C43">
         <v>48.86</v>
@@ -2507,10 +2537,10 @@
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="B44" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="C44">
         <v>104.55</v>
@@ -2518,10 +2548,10 @@
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="B45" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="C45">
         <v>60.28</v>
@@ -2538,7 +2568,7 @@
         <v>0</v>
       </c>
       <c r="G45" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="I45" s="2">
         <v>0.5</v>
@@ -2546,10 +2576,10 @@
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B46" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="C46">
         <v>120.53</v>
@@ -2567,7 +2597,7 @@
         <v>23.1</v>
       </c>
       <c r="G46" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="I46" s="2">
         <v>0.5</v>
@@ -2575,10 +2605,10 @@
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="B47" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="C47">
         <v>231</v>
@@ -2586,349 +2616,380 @@
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>124</v>
+        <v>305</v>
       </c>
       <c r="B48" t="s">
-        <v>124</v>
+        <v>289</v>
       </c>
       <c r="C48">
-        <v>22.07</v>
-      </c>
-      <c r="G48" t="s">
-        <v>125</v>
+        <v>64.73</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>307</v>
+        <v>114</v>
       </c>
       <c r="B49" t="s">
-        <v>291</v>
+        <v>114</v>
       </c>
       <c r="C49">
-        <v>64.73</v>
+        <v>102.48</v>
+      </c>
+      <c r="D49">
+        <f>E49/(1+I49)+F49</f>
+        <v>73.733333333333334</v>
+      </c>
+      <c r="E49">
+        <f>7.9*14</f>
+        <v>110.60000000000001</v>
+      </c>
+      <c r="F49">
+        <v>0</v>
+      </c>
+      <c r="G49" t="s">
+        <v>422</v>
+      </c>
+      <c r="I49" s="2">
+        <v>0.5</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>114</v>
+        <v>261</v>
       </c>
       <c r="B50" t="s">
-        <v>114</v>
+        <v>261</v>
       </c>
       <c r="C50">
-        <v>102.48</v>
+        <v>109.4</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>263</v>
+        <v>66</v>
       </c>
       <c r="B51" t="s">
-        <v>263</v>
+        <v>66</v>
       </c>
       <c r="C51">
-        <v>109.4</v>
+        <v>9.86</v>
+      </c>
+      <c r="D51">
+        <f>1000/64</f>
+        <v>15.625</v>
+      </c>
+      <c r="E51">
+        <f>1000/64</f>
+        <v>15.625</v>
+      </c>
+      <c r="F51">
+        <v>0</v>
+      </c>
+      <c r="G51" t="s">
+        <v>357</v>
+      </c>
+      <c r="I51" s="2">
+        <v>0.65</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>66</v>
+        <v>237</v>
       </c>
       <c r="B52" t="s">
-        <v>66</v>
+        <v>238</v>
       </c>
       <c r="C52">
-        <v>9.86</v>
-      </c>
-      <c r="D52">
-        <f>1000/64</f>
-        <v>15.625</v>
-      </c>
-      <c r="E52">
-        <f>1000/64</f>
-        <v>15.625</v>
-      </c>
-      <c r="F52">
-        <v>0</v>
-      </c>
-      <c r="G52" t="s">
-        <v>359</v>
-      </c>
-      <c r="I52" s="2">
-        <v>0.65</v>
+        <v>5.21</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>239</v>
+        <v>204</v>
       </c>
       <c r="B53" t="s">
-        <v>240</v>
+        <v>166</v>
       </c>
       <c r="C53">
-        <v>5.21</v>
+        <v>137.47</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>206</v>
+        <v>249</v>
       </c>
       <c r="B54" t="s">
-        <v>168</v>
+        <v>250</v>
       </c>
       <c r="C54">
-        <v>137.47</v>
+        <v>116.54</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>251</v>
+        <v>280</v>
       </c>
       <c r="B55" t="s">
-        <v>252</v>
+        <v>129</v>
       </c>
       <c r="C55">
-        <v>116.54</v>
+        <v>166.32</v>
+      </c>
+      <c r="D55">
+        <f>(7.5*35+50/2.4+10/2.4)/1.1/1.1/1.1+36/2.4</f>
+        <v>231.00300525920352</v>
+      </c>
+      <c r="E55">
+        <f>(7.5*35+50/2.4+10/2.4)/1.1/1.1/1.1</f>
+        <v>216.00300525920352</v>
+      </c>
+      <c r="F55">
+        <f>36/2.4</f>
+        <v>15</v>
+      </c>
+      <c r="G55" t="s">
+        <v>371</v>
+      </c>
+      <c r="I55" s="2">
+        <v>0.5</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>282</v>
+        <v>15</v>
       </c>
       <c r="B56" t="s">
-        <v>131</v>
+        <v>16</v>
       </c>
       <c r="C56">
-        <v>166.32</v>
-      </c>
-      <c r="D56">
-        <f>(7.5*35+50/2.4+10/2.4)/1.1/1.1/1.1+36/2.4</f>
-        <v>231.00300525920352</v>
-      </c>
-      <c r="E56">
-        <f>(7.5*35+50/2.4+10/2.4)/1.1/1.1/1.1</f>
-        <v>216.00300525920352</v>
-      </c>
-      <c r="F56">
-        <f>36/2.4</f>
-        <v>15</v>
-      </c>
-      <c r="G56" t="s">
-        <v>373</v>
-      </c>
-      <c r="I56" s="2">
-        <v>0.5</v>
+        <v>52.45</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>15</v>
+        <v>58</v>
       </c>
       <c r="B57" t="s">
-        <v>16</v>
+        <v>59</v>
       </c>
       <c r="C57">
-        <v>52.45</v>
+        <v>196.78</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>58</v>
+        <v>312</v>
       </c>
       <c r="B58" t="s">
-        <v>59</v>
+        <v>309</v>
       </c>
       <c r="C58">
-        <v>196.78</v>
+        <v>34.5</v>
+      </c>
+      <c r="D58">
+        <v>42</v>
+      </c>
+      <c r="E58">
+        <v>42</v>
+      </c>
+      <c r="F58">
+        <v>0</v>
+      </c>
+      <c r="G58" t="s">
+        <v>343</v>
+      </c>
+      <c r="I58" s="2">
+        <v>0.4</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>314</v>
+        <v>286</v>
       </c>
       <c r="B59" t="s">
-        <v>311</v>
+        <v>286</v>
       </c>
       <c r="C59">
-        <v>34.5</v>
-      </c>
-      <c r="D59">
-        <v>42</v>
-      </c>
-      <c r="E59">
-        <v>42</v>
-      </c>
-      <c r="F59">
-        <v>0</v>
-      </c>
-      <c r="G59" t="s">
-        <v>345</v>
-      </c>
-      <c r="I59" s="2">
-        <v>0.4</v>
+        <v>16</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>288</v>
+        <v>265</v>
       </c>
       <c r="B60" t="s">
-        <v>288</v>
+        <v>266</v>
       </c>
       <c r="C60">
-        <v>16</v>
+        <v>32.35</v>
+      </c>
+      <c r="D60">
+        <f>3*17</f>
+        <v>51</v>
+      </c>
+      <c r="E60">
+        <f>3*17</f>
+        <v>51</v>
+      </c>
+      <c r="F60">
+        <v>0</v>
+      </c>
+      <c r="G60" t="s">
+        <v>358</v>
+      </c>
+      <c r="I60" s="2">
+        <v>0.65</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>267</v>
+        <v>277</v>
       </c>
       <c r="B61" t="s">
-        <v>268</v>
+        <v>2</v>
       </c>
       <c r="C61">
-        <v>32.35</v>
-      </c>
-      <c r="D61">
-        <f>3*17</f>
-        <v>51</v>
-      </c>
-      <c r="E61">
-        <f>3*17</f>
-        <v>51</v>
-      </c>
-      <c r="F61">
-        <v>0</v>
-      </c>
-      <c r="G61" t="s">
-        <v>360</v>
-      </c>
-      <c r="I61" s="2">
-        <v>0.65</v>
+        <v>71.25</v>
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>279</v>
+        <v>32</v>
       </c>
       <c r="B62" t="s">
-        <v>2</v>
+        <v>33</v>
       </c>
       <c r="C62">
-        <v>71.25</v>
+        <v>12.97</v>
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>32</v>
+        <v>13</v>
       </c>
       <c r="B63" t="s">
-        <v>33</v>
+        <v>14</v>
       </c>
       <c r="C63">
-        <v>12.97</v>
+        <v>33.799999999999997</v>
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>13</v>
+        <v>256</v>
       </c>
       <c r="B64" t="s">
-        <v>14</v>
+        <v>115</v>
       </c>
       <c r="C64">
-        <v>33.799999999999997</v>
+        <v>1019.97</v>
+      </c>
+      <c r="D64">
+        <f>((30+1)*27+95+30)*1000/700</f>
+        <v>1374.2857142857142</v>
+      </c>
+      <c r="E64">
+        <f>((30+1)*27)*1000/700</f>
+        <v>1195.7142857142858</v>
+      </c>
+      <c r="F64">
+        <f>(95+30)*1000/700</f>
+        <v>178.57142857142858</v>
+      </c>
+      <c r="G64" t="s">
+        <v>383</v>
+      </c>
+      <c r="I64" s="2">
+        <v>0.5</v>
       </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>258</v>
+        <v>181</v>
       </c>
       <c r="B65" t="s">
-        <v>115</v>
+        <v>154</v>
       </c>
       <c r="C65">
-        <v>1019.97</v>
-      </c>
-      <c r="D65">
-        <f>((30+1)*27+95+30)*1000/700</f>
-        <v>1374.2857142857142</v>
-      </c>
-      <c r="E65">
-        <f>((30+1)*27)*1000/700</f>
-        <v>1195.7142857142858</v>
-      </c>
-      <c r="F65">
-        <f>(95+30)*1000/700</f>
-        <v>178.57142857142858</v>
-      </c>
-      <c r="G65" t="s">
-        <v>385</v>
-      </c>
-      <c r="I65" s="2">
-        <v>0.5</v>
+        <v>108.7</v>
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>183</v>
+        <v>82</v>
       </c>
       <c r="B66" t="s">
-        <v>156</v>
+        <v>83</v>
       </c>
       <c r="C66">
-        <v>108.7</v>
+        <v>98.32</v>
+      </c>
+      <c r="G66" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>82</v>
+        <v>252</v>
       </c>
       <c r="B67" t="s">
-        <v>83</v>
+        <v>254</v>
       </c>
       <c r="C67">
-        <v>98.32</v>
-      </c>
-      <c r="G67" t="s">
-        <v>84</v>
+        <v>252.94</v>
       </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>254</v>
+        <v>315</v>
       </c>
       <c r="B68" t="s">
-        <v>256</v>
+        <v>314</v>
       </c>
       <c r="C68">
-        <v>252.94</v>
+        <v>16.11</v>
+      </c>
+      <c r="D68">
+        <f>(730*12-2600)/284</f>
+        <v>21.690140845070424</v>
+      </c>
+      <c r="E68">
+        <f>(730*12-2600)/284</f>
+        <v>21.690140845070424</v>
+      </c>
+      <c r="F68">
+        <v>0</v>
+      </c>
+      <c r="G68" t="s">
+        <v>320</v>
+      </c>
+      <c r="I68" s="2">
+        <v>0.5</v>
       </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>317</v>
+        <v>377</v>
       </c>
       <c r="B69" t="s">
-        <v>316</v>
+        <v>378</v>
       </c>
       <c r="C69">
-        <v>16.11</v>
+        <v>75.62</v>
       </c>
       <c r="D69">
-        <f>(730*12-2600)/284</f>
-        <v>21.690140845070424</v>
+        <f>(14*780-1500)/122</f>
+        <v>77.213114754098356</v>
       </c>
       <c r="E69">
-        <f>(730*12-2600)/284</f>
-        <v>21.690140845070424</v>
+        <f>(14*780-1500)/122</f>
+        <v>77.213114754098356</v>
       </c>
       <c r="F69">
         <v>0</v>
       </c>
       <c r="G69" t="s">
-        <v>322</v>
+        <v>379</v>
       </c>
       <c r="I69" s="2">
         <v>0.5</v>
@@ -2936,321 +2997,321 @@
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>379</v>
+        <v>363</v>
       </c>
       <c r="B70" t="s">
-        <v>380</v>
+        <v>364</v>
       </c>
       <c r="C70">
-        <v>75.62</v>
+        <v>172.86</v>
       </c>
       <c r="D70">
-        <f>(14*780-1500)/122</f>
-        <v>77.213114754098356</v>
+        <f>8.5*20</f>
+        <v>170</v>
       </c>
       <c r="E70">
-        <f>(14*780-1500)/122</f>
-        <v>77.213114754098356</v>
+        <f>8.5*20</f>
+        <v>170</v>
       </c>
       <c r="F70">
         <v>0</v>
       </c>
       <c r="G70" t="s">
-        <v>381</v>
+        <v>366</v>
       </c>
       <c r="I70" s="2">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>365</v>
+        <v>78</v>
       </c>
       <c r="B71" t="s">
-        <v>366</v>
+        <v>77</v>
       </c>
       <c r="C71">
-        <v>172.86</v>
-      </c>
-      <c r="D71">
-        <f>8.5*20</f>
-        <v>170</v>
-      </c>
-      <c r="E71">
-        <f>8.5*20</f>
-        <v>170</v>
-      </c>
-      <c r="F71">
-        <v>0</v>
-      </c>
-      <c r="G71" t="s">
-        <v>368</v>
-      </c>
-      <c r="I71" s="2">
-        <v>0.55000000000000004</v>
+        <v>42.89</v>
       </c>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>78</v>
+        <v>45</v>
       </c>
       <c r="B72" t="s">
-        <v>77</v>
+        <v>46</v>
       </c>
       <c r="C72">
-        <v>42.89</v>
+        <v>79.61</v>
+      </c>
+      <c r="G72" t="s">
+        <v>359</v>
       </c>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>45</v>
+        <v>118</v>
       </c>
       <c r="B73" t="s">
-        <v>46</v>
+        <v>119</v>
       </c>
       <c r="C73">
-        <v>79.61</v>
+        <v>144.28</v>
       </c>
       <c r="G73" t="s">
-        <v>361</v>
+        <v>120</v>
       </c>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>118</v>
+        <v>53</v>
       </c>
       <c r="B74" t="s">
-        <v>119</v>
+        <v>53</v>
       </c>
       <c r="C74">
-        <v>144.28</v>
-      </c>
-      <c r="G74" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="75" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="B75" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="C75" s="3">
         <v>17.239999999999998</v>
       </c>
-      <c r="D75" s="3">
+      <c r="D74">
         <v>22</v>
       </c>
-      <c r="E75" s="3">
+      <c r="E74">
         <v>22</v>
       </c>
-      <c r="F75" s="3">
+      <c r="F74">
         <v>0</v>
       </c>
-      <c r="H75" s="4"/>
-      <c r="I75" s="4">
+      <c r="H74"/>
+      <c r="I74">
         <v>0.65</v>
       </c>
     </row>
-    <row r="76" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="3" t="s">
-        <v>290</v>
-      </c>
-      <c r="B76" s="3" t="s">
-        <v>290</v>
-      </c>
-      <c r="C76" s="3">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>288</v>
+      </c>
+      <c r="B75" t="s">
+        <v>288</v>
+      </c>
+      <c r="C75">
         <v>21.59</v>
       </c>
-      <c r="D76" s="3">
+      <c r="D75">
         <f>1.8*12+1</f>
         <v>22.6</v>
       </c>
-      <c r="E76" s="3">
+      <c r="E75">
         <f>1.8*12</f>
         <v>21.6</v>
       </c>
-      <c r="F76" s="3">
+      <c r="F75">
         <v>1</v>
       </c>
-      <c r="G76" s="3" t="s">
-        <v>352</v>
-      </c>
-      <c r="H76" s="4"/>
-      <c r="I76" s="4">
+      <c r="G75" t="s">
+        <v>350</v>
+      </c>
+      <c r="H75"/>
+      <c r="I75">
         <v>0.6</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>388</v>
+      </c>
+      <c r="B76" t="s">
+        <v>388</v>
+      </c>
+      <c r="C76">
+        <v>154.29</v>
+      </c>
+      <c r="D76">
+        <f>14000/86+700/86</f>
+        <v>170.93023255813952</v>
+      </c>
+      <c r="E76">
+        <f>14000/86+700/86</f>
+        <v>170.93023255813952</v>
+      </c>
+      <c r="F76">
+        <v>0</v>
+      </c>
+      <c r="G76" t="s">
+        <v>390</v>
+      </c>
+      <c r="I76" s="2">
+        <v>0.4</v>
       </c>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>390</v>
+        <v>12</v>
       </c>
       <c r="B77" t="s">
-        <v>390</v>
+        <v>12</v>
       </c>
       <c r="C77">
-        <v>154.29</v>
+        <v>155.36000000000001</v>
       </c>
       <c r="D77">
-        <f>14000/86+700/86</f>
-        <v>170.93023255813952</v>
+        <f>13.8*15</f>
+        <v>207</v>
       </c>
       <c r="E77">
-        <f>14000/86+700/86</f>
-        <v>170.93023255813952</v>
+        <f>13.8*15</f>
+        <v>207</v>
       </c>
       <c r="F77">
         <v>0</v>
       </c>
       <c r="G77" t="s">
-        <v>392</v>
+        <v>372</v>
       </c>
       <c r="I77" s="2">
-        <v>0.4</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>12</v>
+        <v>200</v>
       </c>
       <c r="B78" t="s">
-        <v>12</v>
+        <v>168</v>
       </c>
       <c r="C78">
-        <v>155.36000000000001</v>
-      </c>
-      <c r="D78">
-        <f>13.8*15</f>
-        <v>207</v>
-      </c>
-      <c r="E78">
-        <f>13.8*15</f>
-        <v>207</v>
-      </c>
-      <c r="F78">
-        <v>0</v>
-      </c>
-      <c r="G78" t="s">
-        <v>374</v>
-      </c>
-      <c r="I78" s="2">
-        <v>0.6</v>
+        <v>71.39</v>
       </c>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>202</v>
+        <v>34</v>
       </c>
       <c r="B79" t="s">
-        <v>170</v>
+        <v>35</v>
       </c>
       <c r="C79">
-        <v>71.39</v>
+        <v>51.1</v>
       </c>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>34</v>
+        <v>190</v>
       </c>
       <c r="B80" t="s">
-        <v>35</v>
+        <v>137</v>
       </c>
       <c r="C80">
-        <v>51.1</v>
+        <v>171.59</v>
       </c>
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>192</v>
+        <v>17</v>
       </c>
       <c r="B81" t="s">
-        <v>139</v>
+        <v>18</v>
       </c>
       <c r="C81">
-        <v>171.59</v>
+        <v>17.329999999999998</v>
       </c>
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="B82" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="C82">
-        <v>17.329999999999998</v>
+        <v>412.12</v>
       </c>
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>25</v>
+        <v>101</v>
       </c>
       <c r="B83" t="s">
-        <v>26</v>
+        <v>102</v>
       </c>
       <c r="C83">
-        <v>412.12</v>
-      </c>
-    </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A84" t="s">
-        <v>101</v>
-      </c>
-      <c r="B84" t="s">
-        <v>102</v>
-      </c>
-      <c r="C84">
         <v>116.32</v>
       </c>
     </row>
-    <row r="85" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A85" s="3" t="s">
-        <v>187</v>
-      </c>
-      <c r="B85" s="3" t="s">
-        <v>136</v>
-      </c>
-      <c r="C85" s="3">
+    <row r="84" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A84" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="B84" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="C84" s="3">
         <v>40.46</v>
       </c>
-      <c r="H85" s="4"/>
-      <c r="I85" s="4"/>
+      <c r="H84" s="4"/>
+      <c r="I84" s="4"/>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>247</v>
+      </c>
+      <c r="B85" t="s">
+        <v>248</v>
+      </c>
+      <c r="C85">
+        <v>110.62</v>
+      </c>
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>249</v>
+        <v>19</v>
       </c>
       <c r="B86" t="s">
-        <v>250</v>
+        <v>20</v>
       </c>
       <c r="C86">
-        <v>110.62</v>
+        <v>61.54</v>
+      </c>
+      <c r="D86">
+        <f>(8500*14-30000)/1228</f>
+        <v>72.475570032573287</v>
+      </c>
+      <c r="E86">
+        <f>(8500*14-30000)/1228</f>
+        <v>72.475570032573287</v>
+      </c>
+      <c r="F86">
+        <v>0</v>
+      </c>
+      <c r="G86" t="s">
+        <v>362</v>
+      </c>
+      <c r="I86" s="2">
+        <v>0.5</v>
       </c>
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>19</v>
+        <v>229</v>
       </c>
       <c r="B87" t="s">
-        <v>20</v>
+        <v>230</v>
       </c>
       <c r="C87">
-        <v>61.54</v>
+        <v>63.38</v>
       </c>
       <c r="D87">
-        <f>(8500*14-30000)/1228</f>
-        <v>72.475570032573287</v>
+        <f>E87/(1+I87)+F87</f>
+        <v>52.699999999999996</v>
       </c>
       <c r="E87">
-        <f>(8500*14-30000)/1228</f>
-        <v>72.475570032573287</v>
+        <f>5.27*15</f>
+        <v>79.05</v>
       </c>
       <c r="F87">
         <v>0</v>
       </c>
       <c r="G87" t="s">
-        <v>364</v>
+        <v>414</v>
       </c>
       <c r="I87" s="2">
         <v>0.5</v>
@@ -3258,1490 +3319,1570 @@
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>231</v>
+        <v>72</v>
       </c>
       <c r="B88" t="s">
-        <v>232</v>
+        <v>73</v>
       </c>
       <c r="C88">
-        <v>63.38</v>
+        <v>194.93</v>
       </c>
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>72</v>
+        <v>306</v>
       </c>
       <c r="B89" t="s">
-        <v>73</v>
+        <v>287</v>
       </c>
       <c r="C89">
-        <v>194.93</v>
+        <v>63.5</v>
       </c>
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>308</v>
+        <v>70</v>
       </c>
       <c r="B90" t="s">
-        <v>289</v>
+        <v>71</v>
       </c>
       <c r="C90">
-        <v>63.5</v>
-      </c>
-    </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A91" t="s">
-        <v>70</v>
-      </c>
-      <c r="B91" t="s">
-        <v>71</v>
-      </c>
-      <c r="C91">
         <v>38.24</v>
       </c>
     </row>
-    <row r="92" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A92" s="3" t="s">
+    <row r="91" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A91" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="B92" s="3" t="s">
+      <c r="B91" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="C92" s="3">
+      <c r="C91" s="3">
         <v>86.65</v>
       </c>
-      <c r="D92" s="3">
+      <c r="D91" s="3">
         <f>5.4*20</f>
         <v>108</v>
       </c>
-      <c r="E92" s="3">
+      <c r="E91" s="3">
         <f>5.4*20</f>
         <v>108</v>
       </c>
-      <c r="F92" s="3">
+      <c r="F91" s="3">
         <v>0</v>
       </c>
-      <c r="G92" s="3" t="s">
-        <v>367</v>
-      </c>
-      <c r="H92" s="4"/>
-      <c r="I92" s="4">
+      <c r="G91" s="3" t="s">
+        <v>365</v>
+      </c>
+      <c r="H91" s="4"/>
+      <c r="I91" s="4">
         <v>0.55000000000000004</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>300</v>
+      </c>
+      <c r="B92" t="s">
+        <v>297</v>
+      </c>
+      <c r="C92">
+        <v>19.22</v>
+      </c>
+      <c r="D92">
+        <f>(8.4+240/117.5+120/117.45*12.5)</f>
+        <v>23.213945273226273</v>
+      </c>
+      <c r="E92">
+        <f>(120/117.45*12.5)</f>
+        <v>12.771392081736909</v>
+      </c>
+      <c r="F92">
+        <f>(8.4+240/117.5)</f>
+        <v>10.442553191489361</v>
+      </c>
+      <c r="G92" t="s">
+        <v>346</v>
+      </c>
+      <c r="I92" s="2">
+        <v>0.5</v>
       </c>
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>302</v>
+        <v>74</v>
       </c>
       <c r="B93" t="s">
-        <v>299</v>
+        <v>75</v>
       </c>
       <c r="C93">
-        <v>19.22</v>
+        <v>29.07</v>
       </c>
       <c r="D93">
-        <f>(8.4+240/117.5+120/117.45*12.5)</f>
-        <v>23.213945273226273</v>
+        <f>E93/(1+I93)+F93</f>
+        <v>30.765372168284792</v>
       </c>
       <c r="E93">
-        <f>(120/117.45*12.5)</f>
-        <v>12.771392081736909</v>
+        <f>2.85*15</f>
+        <v>42.75</v>
       </c>
       <c r="F93">
-        <f>(8.4+240/117.5)</f>
-        <v>10.442553191489361</v>
+        <f>700/309</f>
+        <v>2.2653721682847898</v>
       </c>
       <c r="G93" t="s">
-        <v>348</v>
+        <v>415</v>
       </c>
       <c r="I93" s="2">
         <v>0.5</v>
       </c>
     </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A94" t="s">
-        <v>74</v>
-      </c>
-      <c r="B94" t="s">
-        <v>75</v>
-      </c>
-      <c r="C94">
-        <v>29.07</v>
-      </c>
-    </row>
-    <row r="95" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A95" s="3" t="s">
-        <v>203</v>
-      </c>
-      <c r="B95" s="3" t="s">
-        <v>169</v>
-      </c>
-      <c r="C95" s="3">
+    <row r="94" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A94" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="B94" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="C94" s="3">
         <v>172.36</v>
       </c>
-      <c r="H95" s="4"/>
-      <c r="I95" s="4"/>
-    </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A96" t="s">
-        <v>186</v>
-      </c>
-      <c r="B96" t="s">
-        <v>140</v>
-      </c>
-      <c r="C96">
+      <c r="H94" s="4"/>
+      <c r="I94" s="4"/>
+    </row>
+    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>184</v>
+      </c>
+      <c r="B95" t="s">
+        <v>138</v>
+      </c>
+      <c r="C95">
         <v>41.6</v>
       </c>
     </row>
-    <row r="97" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A97" s="3" t="s">
-        <v>191</v>
-      </c>
-      <c r="B97" s="3" t="s">
-        <v>159</v>
-      </c>
-      <c r="C97" s="3">
+    <row r="96" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A96" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="B96" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="C96" s="3">
         <v>163.34</v>
       </c>
-      <c r="H97" s="4"/>
-      <c r="I97" s="4"/>
+      <c r="H96" s="4"/>
+      <c r="I96" s="4"/>
+    </row>
+    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>155</v>
+      </c>
+      <c r="B97" t="s">
+        <v>42</v>
+      </c>
+      <c r="C97">
+        <v>162.4</v>
+      </c>
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>157</v>
+        <v>385</v>
       </c>
       <c r="B98" t="s">
-        <v>42</v>
+        <v>384</v>
       </c>
       <c r="C98">
-        <v>162.4</v>
-      </c>
-    </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A99" t="s">
-        <v>387</v>
-      </c>
-      <c r="B99" t="s">
-        <v>386</v>
-      </c>
-      <c r="C99">
         <v>16.489999999999998</v>
       </c>
-      <c r="D99">
+      <c r="D98">
         <f>(1400*10*0.5+1400*12*0.25+1700*12*0.25-4409)/435</f>
         <v>27.335632183908046</v>
       </c>
-      <c r="E99">
+      <c r="E98">
         <f>(1400*10*0.5+1400*12*0.25+1700*12*0.25-4409)/435</f>
         <v>27.335632183908046</v>
       </c>
-      <c r="F99">
+      <c r="F98">
         <v>0</v>
       </c>
-      <c r="G99" t="s">
-        <v>388</v>
-      </c>
-      <c r="I99" s="2">
+      <c r="G98" t="s">
+        <v>386</v>
+      </c>
+      <c r="I98" s="2">
         <v>0.65</v>
       </c>
     </row>
-    <row r="100" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A100" s="3" t="s">
+    <row r="99" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A99" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="B100" s="3" t="s">
+      <c r="B99" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="C100" s="3">
+      <c r="C99" s="3">
         <v>123.68</v>
       </c>
-      <c r="G100" s="3" t="s">
+      <c r="G99" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="H100" s="4"/>
-      <c r="I100" s="4"/>
+      <c r="H99" s="4"/>
+      <c r="I99" s="4"/>
+    </row>
+    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>209</v>
+      </c>
+      <c r="B100" t="s">
+        <v>149</v>
+      </c>
+      <c r="C100">
+        <v>37.4</v>
+      </c>
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>211</v>
+        <v>251</v>
       </c>
       <c r="B101" t="s">
-        <v>151</v>
+        <v>253</v>
       </c>
       <c r="C101">
-        <v>37.4</v>
+        <v>52.74</v>
       </c>
     </row>
     <row r="102" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>253</v>
+        <v>36</v>
       </c>
       <c r="B102" t="s">
-        <v>255</v>
+        <v>37</v>
       </c>
       <c r="C102">
-        <v>52.74</v>
+        <v>148.25</v>
       </c>
     </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>36</v>
+        <v>207</v>
       </c>
       <c r="B103" t="s">
-        <v>37</v>
+        <v>152</v>
       </c>
       <c r="C103">
-        <v>148.25</v>
+        <v>91.86</v>
+      </c>
+      <c r="D103">
+        <f>40000/7710+3.6*25</f>
+        <v>95.188067444876779</v>
+      </c>
+      <c r="E103">
+        <f>3.6*25</f>
+        <v>90</v>
+      </c>
+      <c r="F103">
+        <f>40000/7710</f>
+        <v>5.1880674448767836</v>
+      </c>
+      <c r="G103" t="s">
+        <v>355</v>
+      </c>
+      <c r="I103" s="2">
+        <v>0.5</v>
       </c>
     </row>
     <row r="104" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>209</v>
+        <v>232</v>
       </c>
       <c r="B104" t="s">
-        <v>154</v>
+        <v>131</v>
       </c>
       <c r="C104">
-        <v>91.86</v>
+        <v>43.9</v>
       </c>
       <c r="D104">
-        <f>40000/7710+3.6*25</f>
-        <v>95.188067444876779</v>
+        <f>E104/(I104+1)</f>
+        <v>14.235294117647062</v>
       </c>
       <c r="E104">
-        <f>3.6*25</f>
-        <v>90</v>
+        <f>330/300*22</f>
+        <v>24.200000000000003</v>
       </c>
       <c r="F104">
-        <f>40000/7710</f>
-        <v>5.1880674448767836</v>
+        <v>0</v>
       </c>
       <c r="G104" t="s">
-        <v>357</v>
-      </c>
-      <c r="I104" s="2">
-        <v>0.5</v>
+        <v>410</v>
+      </c>
+      <c r="H104"/>
+      <c r="I104" s="9">
+        <v>0.7</v>
       </c>
     </row>
     <row r="105" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>234</v>
+        <v>199</v>
       </c>
       <c r="B105" t="s">
-        <v>133</v>
+        <v>158</v>
       </c>
       <c r="C105">
-        <v>43.9</v>
-      </c>
-      <c r="D105">
-        <f>E105/(I105+1)</f>
-        <v>14.235294117647062</v>
-      </c>
-      <c r="E105">
-        <f>330/300*22</f>
-        <v>24.200000000000003</v>
-      </c>
-      <c r="F105">
-        <v>0</v>
-      </c>
-      <c r="G105" t="s">
-        <v>412</v>
-      </c>
-      <c r="H105"/>
-      <c r="I105" s="9">
-        <v>0.7</v>
+        <v>303.67</v>
       </c>
     </row>
     <row r="106" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>201</v>
+        <v>80</v>
       </c>
       <c r="B106" t="s">
-        <v>160</v>
+        <v>79</v>
       </c>
       <c r="C106">
-        <v>303.67</v>
+        <v>66.83</v>
       </c>
     </row>
     <row r="107" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>80</v>
+        <v>196</v>
       </c>
       <c r="B107" t="s">
-        <v>79</v>
+        <v>144</v>
       </c>
       <c r="C107">
-        <v>66.83</v>
+        <v>166.5</v>
       </c>
     </row>
     <row r="108" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>198</v>
+        <v>177</v>
       </c>
       <c r="B108" t="s">
-        <v>146</v>
+        <v>176</v>
       </c>
       <c r="C108">
-        <v>166.5</v>
-      </c>
-    </row>
-    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A109" t="s">
-        <v>179</v>
-      </c>
-      <c r="B109" t="s">
-        <v>178</v>
-      </c>
-      <c r="C109">
         <v>61.55</v>
       </c>
     </row>
-    <row r="110" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A110" s="3" t="s">
+    <row r="109" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A109" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="B110" s="3" t="s">
+      <c r="B109" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="C110" s="3">
+      <c r="C109" s="3">
         <v>226.24</v>
       </c>
-      <c r="D110" s="3">
+      <c r="D109" s="3">
         <f>5000/600+6*25</f>
         <v>158.33333333333334</v>
       </c>
-      <c r="E110" s="3">
+      <c r="E109" s="3">
         <f>6*25</f>
         <v>150</v>
       </c>
-      <c r="F110" s="3">
+      <c r="F109" s="3">
         <f>5000/600</f>
         <v>8.3333333333333339</v>
       </c>
-      <c r="G110" s="3" t="s">
-        <v>375</v>
-      </c>
-      <c r="H110" s="4"/>
-      <c r="I110" s="4">
+      <c r="G109" s="3" t="s">
+        <v>373</v>
+      </c>
+      <c r="H109" s="4"/>
+      <c r="I109" s="4">
         <v>0.5</v>
+      </c>
+    </row>
+    <row r="110" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>91</v>
+      </c>
+      <c r="B110" t="s">
+        <v>92</v>
+      </c>
+      <c r="C110">
+        <v>63.95</v>
       </c>
     </row>
     <row r="111" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>91</v>
+        <v>226</v>
       </c>
       <c r="B111" t="s">
-        <v>92</v>
+        <v>227</v>
       </c>
       <c r="C111">
-        <v>63.95</v>
-      </c>
-    </row>
-    <row r="112" spans="1:9" x14ac:dyDescent="0.25">
+        <v>7.94</v>
+      </c>
+    </row>
+    <row r="112" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
+        <v>225</v>
+      </c>
+      <c r="B112" t="s">
         <v>228</v>
       </c>
-      <c r="B112" t="s">
-        <v>229</v>
-      </c>
       <c r="C112">
-        <v>7.94</v>
-      </c>
-    </row>
-    <row r="113" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>4.34</v>
+      </c>
+      <c r="D112">
+        <v>5</v>
+      </c>
+      <c r="E112">
+        <v>5</v>
+      </c>
+      <c r="F112">
+        <v>0</v>
+      </c>
+      <c r="G112" t="s">
+        <v>367</v>
+      </c>
+      <c r="I112" s="2">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="113" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>227</v>
+        <v>381</v>
       </c>
       <c r="B113" t="s">
-        <v>230</v>
+        <v>381</v>
       </c>
       <c r="C113">
-        <v>4.34</v>
+        <v>100.15</v>
       </c>
       <c r="D113">
-        <v>5</v>
-      </c>
-      <c r="E113">
-        <v>5</v>
-      </c>
-      <c r="F113">
-        <v>0</v>
-      </c>
-      <c r="G113" t="s">
-        <v>369</v>
-      </c>
-      <c r="I113" s="2">
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="114" spans="1:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A114" t="s">
-        <v>383</v>
-      </c>
-      <c r="B114" t="s">
-        <v>383</v>
-      </c>
-      <c r="C114">
-        <v>100.15</v>
-      </c>
-      <c r="D114">
         <f>4*20+9</f>
         <v>89</v>
       </c>
-      <c r="E114">
+      <c r="E113">
         <f>4*20</f>
         <v>80</v>
       </c>
-      <c r="F114">
+      <c r="F113">
         <v>9</v>
       </c>
+      <c r="G113" t="s">
+        <v>382</v>
+      </c>
+      <c r="I113" s="2">
+        <v>0.65</v>
+      </c>
+    </row>
+    <row r="114" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
+        <v>125</v>
+      </c>
+      <c r="B114" t="s">
+        <v>124</v>
+      </c>
+      <c r="C114">
+        <v>45.61</v>
+      </c>
       <c r="G114" t="s">
-        <v>384</v>
-      </c>
-      <c r="I114" s="2">
-        <v>0.65</v>
+        <v>126</v>
       </c>
     </row>
     <row r="115" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>127</v>
+        <v>310</v>
       </c>
       <c r="B115" t="s">
-        <v>126</v>
+        <v>307</v>
       </c>
       <c r="C115">
-        <v>45.61</v>
+        <v>35.119999999999997</v>
+      </c>
+      <c r="D115">
+        <f>10*1375/313</f>
+        <v>43.929712460063897</v>
+      </c>
+      <c r="E115">
+        <f>10*1375/313</f>
+        <v>43.929712460063897</v>
+      </c>
+      <c r="F115">
+        <v>0</v>
       </c>
       <c r="G115" t="s">
-        <v>128</v>
+        <v>321</v>
+      </c>
+      <c r="I115" s="2">
+        <v>0.4</v>
       </c>
     </row>
     <row r="116" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>312</v>
+        <v>273</v>
       </c>
       <c r="B116" t="s">
-        <v>309</v>
+        <v>274</v>
       </c>
       <c r="C116">
-        <v>35.119999999999997</v>
+        <v>9.43</v>
       </c>
       <c r="D116">
-        <f>10*1375/313</f>
-        <v>43.929712460063897</v>
+        <f>(875*10-5000+360*0.5)/286</f>
+        <v>13.741258741258742</v>
       </c>
       <c r="E116">
-        <f>10*1375/313</f>
-        <v>43.929712460063897</v>
+        <f>(875*10-5000+360*0.5)/286</f>
+        <v>13.741258741258742</v>
       </c>
       <c r="F116">
         <v>0</v>
       </c>
       <c r="G116" t="s">
-        <v>323</v>
+        <v>351</v>
       </c>
       <c r="I116" s="2">
-        <v>0.4</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="117" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>275</v>
+        <v>88</v>
       </c>
       <c r="B117" t="s">
-        <v>276</v>
+        <v>87</v>
       </c>
       <c r="C117">
-        <v>9.43</v>
-      </c>
-      <c r="D117">
-        <f>(875*10-5000+360*0.5)/286</f>
-        <v>13.741258741258742</v>
-      </c>
-      <c r="E117">
-        <f>(875*10-5000+360*0.5)/286</f>
-        <v>13.741258741258742</v>
-      </c>
-      <c r="F117">
-        <v>0</v>
-      </c>
-      <c r="G117" t="s">
-        <v>353</v>
-      </c>
-      <c r="I117" s="2">
-        <v>0.6</v>
+        <v>186.99</v>
       </c>
     </row>
     <row r="118" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>88</v>
+        <v>40</v>
       </c>
       <c r="B118" t="s">
-        <v>87</v>
+        <v>41</v>
       </c>
       <c r="C118">
-        <v>186.99</v>
+        <v>61.67</v>
       </c>
     </row>
     <row r="119" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>40</v>
+        <v>290</v>
       </c>
       <c r="B119" t="s">
-        <v>41</v>
+        <v>285</v>
       </c>
       <c r="C119">
-        <v>61.67</v>
-      </c>
-    </row>
-    <row r="120" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A120" t="s">
-        <v>292</v>
-      </c>
-      <c r="B120" t="s">
-        <v>287</v>
-      </c>
-      <c r="C120">
         <v>44.8</v>
       </c>
     </row>
-    <row r="121" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A121" s="3" t="s">
-        <v>207</v>
-      </c>
-      <c r="B121" s="3" t="s">
-        <v>395</v>
-      </c>
-      <c r="C121" s="3">
+    <row r="120" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A120" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="B120" s="3" t="s">
+        <v>393</v>
+      </c>
+      <c r="C120" s="3">
         <v>1905.64</v>
       </c>
-      <c r="H121" s="4"/>
-      <c r="I121" s="4"/>
+      <c r="H120" s="4"/>
+      <c r="I120" s="4"/>
+    </row>
+    <row r="121" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A121" t="s">
+        <v>258</v>
+      </c>
+      <c r="B121" t="s">
+        <v>259</v>
+      </c>
+      <c r="C121">
+        <v>29.55</v>
+      </c>
+      <c r="D121">
+        <f>2.8*15</f>
+        <v>42</v>
+      </c>
+      <c r="E121">
+        <f>2.8*15</f>
+        <v>42</v>
+      </c>
+      <c r="F121">
+        <v>0</v>
+      </c>
+      <c r="G121" t="s">
+        <v>323</v>
+      </c>
+      <c r="I121" s="2">
+        <v>0.6</v>
+      </c>
     </row>
     <row r="122" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>260</v>
+        <v>272</v>
       </c>
       <c r="B122" t="s">
-        <v>261</v>
+        <v>81</v>
       </c>
       <c r="C122">
-        <v>29.55</v>
-      </c>
-      <c r="D122">
-        <f>2.8*15</f>
-        <v>42</v>
-      </c>
-      <c r="E122">
-        <f>2.8*15</f>
-        <v>42</v>
-      </c>
-      <c r="F122">
-        <v>0</v>
-      </c>
-      <c r="G122" t="s">
-        <v>325</v>
-      </c>
-      <c r="I122" s="2">
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="123" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+        <v>102.55</v>
+      </c>
+    </row>
+    <row r="123" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>274</v>
+        <v>21</v>
       </c>
       <c r="B123" t="s">
-        <v>81</v>
+        <v>22</v>
       </c>
       <c r="C123">
-        <v>102.55</v>
-      </c>
-    </row>
-    <row r="124" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A124" t="s">
-        <v>21</v>
-      </c>
-      <c r="B124" t="s">
-        <v>22</v>
-      </c>
-      <c r="C124">
         <v>76.5</v>
       </c>
     </row>
-    <row r="125" spans="1:9" s="3" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:9" s="3" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A124" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="B124" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="C124" s="3">
+        <v>62.16</v>
+      </c>
+      <c r="H124" s="4"/>
+      <c r="I124" s="4"/>
+    </row>
+    <row r="125" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A125" s="3" t="s">
-        <v>245</v>
+        <v>86</v>
       </c>
       <c r="B125" s="3" t="s">
-        <v>162</v>
+        <v>85</v>
       </c>
       <c r="C125" s="3">
-        <v>62.16</v>
+        <v>55.89</v>
       </c>
       <c r="H125" s="4"/>
       <c r="I125" s="4"/>
     </row>
-    <row r="126" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A126" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="B126" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="C126" s="3">
-        <v>55.89</v>
-      </c>
-      <c r="H126" s="4"/>
-      <c r="I126" s="4"/>
+    <row r="126" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A126" t="s">
+        <v>239</v>
+      </c>
+      <c r="B126" t="s">
+        <v>240</v>
+      </c>
+      <c r="C126">
+        <v>14.64</v>
+      </c>
     </row>
     <row r="127" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>241</v>
+        <v>369</v>
       </c>
       <c r="B127" t="s">
-        <v>242</v>
+        <v>291</v>
       </c>
       <c r="C127">
-        <v>14.64</v>
-      </c>
-    </row>
-    <row r="128" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A128" t="s">
-        <v>371</v>
-      </c>
-      <c r="B128" t="s">
-        <v>293</v>
-      </c>
-      <c r="C128">
         <v>86.63</v>
       </c>
     </row>
-    <row r="129" spans="1:9" s="3" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A129" s="3" t="s">
-        <v>193</v>
-      </c>
-      <c r="B129" s="3" t="s">
-        <v>172</v>
-      </c>
-      <c r="C129" s="3">
+    <row r="128" spans="1:9" s="3" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A128" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="B128" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="C128" s="3">
         <v>156.4</v>
       </c>
-      <c r="H129" s="4"/>
-      <c r="I129" s="4"/>
+      <c r="H128" s="4"/>
+      <c r="I128" s="4"/>
+    </row>
+    <row r="129" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A129" t="s">
+        <v>139</v>
+      </c>
+      <c r="B129" t="s">
+        <v>139</v>
+      </c>
+      <c r="C129">
+        <v>106.97</v>
+      </c>
     </row>
     <row r="130" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>141</v>
+        <v>220</v>
       </c>
       <c r="B130" t="s">
-        <v>141</v>
+        <v>221</v>
       </c>
       <c r="C130">
-        <v>106.97</v>
+        <v>13.37</v>
+      </c>
+      <c r="D130">
+        <f>16*(97*1.3+18)*(1-35%)*(1-29%)/53</f>
+        <v>20.076120754716985</v>
+      </c>
+      <c r="E130">
+        <f>16*(97*1.3+18)*(1-35%)*(1-29%)/53</f>
+        <v>20.076120754716985</v>
+      </c>
+      <c r="F130">
+        <v>0</v>
+      </c>
+      <c r="G130" t="s">
+        <v>327</v>
+      </c>
+      <c r="I130" s="2">
+        <v>0.6</v>
       </c>
     </row>
     <row r="131" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>222</v>
+        <v>121</v>
       </c>
       <c r="B131" t="s">
-        <v>223</v>
+        <v>122</v>
       </c>
       <c r="C131">
-        <v>13.37</v>
-      </c>
-      <c r="D131">
-        <f>16*(97*1.3+18)*(1-35%)*(1-29%)/53</f>
-        <v>20.076120754716985</v>
-      </c>
-      <c r="E131">
-        <f>16*(97*1.3+18)*(1-35%)*(1-29%)/53</f>
-        <v>20.076120754716985</v>
-      </c>
-      <c r="F131">
-        <v>0</v>
-      </c>
-      <c r="G131" t="s">
-        <v>329</v>
-      </c>
-      <c r="I131" s="2">
-        <v>0.6</v>
+        <v>59.42</v>
       </c>
     </row>
     <row r="132" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>121</v>
+        <v>304</v>
       </c>
       <c r="B132" t="s">
-        <v>122</v>
+        <v>292</v>
       </c>
       <c r="C132">
-        <v>59.42</v>
+        <v>55</v>
       </c>
     </row>
     <row r="133" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>306</v>
+        <v>222</v>
       </c>
       <c r="B133" t="s">
-        <v>294</v>
+        <v>165</v>
       </c>
       <c r="C133">
-        <v>55</v>
+        <v>23.18</v>
       </c>
     </row>
     <row r="134" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>224</v>
+        <v>128</v>
       </c>
       <c r="B134" t="s">
-        <v>167</v>
+        <v>50</v>
       </c>
       <c r="C134">
-        <v>23.18</v>
+        <v>43.36</v>
       </c>
     </row>
     <row r="135" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>130</v>
+        <v>197</v>
       </c>
       <c r="B135" t="s">
-        <v>50</v>
+        <v>140</v>
       </c>
       <c r="C135">
-        <v>43.36</v>
+        <v>119.53</v>
       </c>
     </row>
     <row r="136" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>199</v>
+        <v>8</v>
       </c>
       <c r="B136" t="s">
-        <v>142</v>
+        <v>9</v>
       </c>
       <c r="C136">
-        <v>119.53</v>
+        <v>42.19</v>
       </c>
     </row>
     <row r="137" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>8</v>
+        <v>270</v>
       </c>
       <c r="B137" t="s">
-        <v>9</v>
+        <v>271</v>
       </c>
       <c r="C137">
-        <v>42.19</v>
+        <v>67.55</v>
       </c>
     </row>
     <row r="138" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>272</v>
+        <v>246</v>
       </c>
       <c r="B138" t="s">
-        <v>273</v>
+        <v>90</v>
       </c>
       <c r="C138">
-        <v>67.55</v>
+        <v>14.8</v>
       </c>
     </row>
     <row r="139" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>248</v>
+        <v>223</v>
       </c>
       <c r="B139" t="s">
-        <v>90</v>
+        <v>224</v>
       </c>
       <c r="C139">
-        <v>14.8</v>
-      </c>
+        <v>8.52</v>
+      </c>
+      <c r="H139"/>
+      <c r="I139"/>
     </row>
     <row r="140" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>225</v>
+        <v>255</v>
       </c>
       <c r="B140" t="s">
-        <v>226</v>
+        <v>133</v>
       </c>
       <c r="C140">
-        <v>8.52</v>
-      </c>
-      <c r="H140"/>
-      <c r="I140"/>
+        <v>34.75</v>
+      </c>
     </row>
     <row r="141" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>257</v>
+        <v>192</v>
       </c>
       <c r="B141" t="s">
-        <v>135</v>
+        <v>156</v>
       </c>
       <c r="C141">
-        <v>34.75</v>
+        <v>189.45</v>
       </c>
     </row>
     <row r="142" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B142" t="s">
-        <v>158</v>
+        <v>142</v>
       </c>
       <c r="C142">
-        <v>189.45</v>
+        <v>21.75</v>
       </c>
     </row>
     <row r="143" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>195</v>
+        <v>108</v>
       </c>
       <c r="B143" t="s">
-        <v>144</v>
+        <v>276</v>
       </c>
       <c r="C143">
-        <v>21.75</v>
+        <v>58.56</v>
+      </c>
+      <c r="D143">
+        <f>4.5*10+2</f>
+        <v>47</v>
+      </c>
+      <c r="E143">
+        <f>4.5*10</f>
+        <v>45</v>
+      </c>
+      <c r="F143">
+        <v>2</v>
+      </c>
+      <c r="G143" t="s">
+        <v>352</v>
+      </c>
+      <c r="I143" s="2">
+        <v>0.65</v>
       </c>
     </row>
     <row r="144" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>108</v>
+        <v>43</v>
       </c>
       <c r="B144" t="s">
-        <v>278</v>
+        <v>44</v>
       </c>
       <c r="C144">
-        <v>58.56</v>
-      </c>
-      <c r="D144">
-        <f>4.5*10+2</f>
-        <v>47</v>
-      </c>
-      <c r="E144">
-        <f>4.5*10</f>
-        <v>45</v>
-      </c>
-      <c r="F144">
-        <v>2</v>
-      </c>
-      <c r="G144" t="s">
-        <v>354</v>
-      </c>
-      <c r="I144" s="2">
-        <v>0.65</v>
+        <v>58.66</v>
       </c>
     </row>
     <row r="145" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>43</v>
+        <v>269</v>
       </c>
       <c r="B145" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="C145">
-        <v>58.66</v>
+        <v>97.7</v>
       </c>
     </row>
     <row r="146" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>271</v>
+        <v>56</v>
       </c>
       <c r="B146" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="C146">
-        <v>97.7</v>
+        <v>21.08</v>
+      </c>
+      <c r="D146">
+        <f>(56-14)*(1-23%)/19*17</f>
+        <v>28.935789473684217</v>
+      </c>
+      <c r="E146">
+        <f>(56-14)*(1-23%)/19*17</f>
+        <v>28.935789473684217</v>
+      </c>
+      <c r="F146">
+        <v>0</v>
+      </c>
+      <c r="G146" t="s">
+        <v>360</v>
+      </c>
+      <c r="I146" s="2">
+        <v>0.6</v>
       </c>
     </row>
     <row r="147" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>56</v>
+        <v>245</v>
       </c>
       <c r="B147" t="s">
-        <v>57</v>
+        <v>282</v>
       </c>
       <c r="C147">
-        <v>21.08</v>
+        <v>52.46</v>
       </c>
       <c r="D147">
-        <f>(56-14)*(1-23%)/19*17</f>
-        <v>28.935789473684217</v>
+        <f>2.9*20</f>
+        <v>58</v>
       </c>
       <c r="E147">
-        <f>(56-14)*(1-23%)/19*17</f>
-        <v>28.935789473684217</v>
+        <f>2.9*20</f>
+        <v>58</v>
       </c>
       <c r="F147">
         <v>0</v>
       </c>
       <c r="G147" t="s">
-        <v>362</v>
+        <v>322</v>
       </c>
       <c r="I147" s="2">
-        <v>0.6</v>
+        <v>0.65</v>
       </c>
     </row>
     <row r="148" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>247</v>
+        <v>38</v>
       </c>
       <c r="B148" t="s">
-        <v>284</v>
+        <v>39</v>
       </c>
       <c r="C148">
-        <v>52.46</v>
-      </c>
-      <c r="D148">
-        <f>2.9*20</f>
-        <v>58</v>
-      </c>
-      <c r="E148">
-        <f>2.9*20</f>
-        <v>58</v>
-      </c>
-      <c r="F148">
-        <v>0</v>
-      </c>
-      <c r="G148" t="s">
-        <v>324</v>
-      </c>
-      <c r="I148" s="2">
-        <v>0.65</v>
+        <v>318.2</v>
       </c>
     </row>
     <row r="149" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>38</v>
+        <v>51</v>
       </c>
       <c r="B149" t="s">
-        <v>39</v>
+        <v>52</v>
       </c>
       <c r="C149">
-        <v>318.2</v>
+        <v>26.79</v>
       </c>
     </row>
     <row r="150" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>51</v>
+        <v>104</v>
       </c>
       <c r="B150" t="s">
-        <v>52</v>
+        <v>105</v>
       </c>
       <c r="C150">
-        <v>26.79</v>
+        <v>6.74</v>
+      </c>
+      <c r="G150" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="151" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>104</v>
+        <v>182</v>
       </c>
       <c r="B151" t="s">
-        <v>105</v>
+        <v>76</v>
       </c>
       <c r="C151">
-        <v>6.74</v>
-      </c>
-      <c r="G151" t="s">
-        <v>106</v>
+        <v>43.38</v>
       </c>
     </row>
     <row r="152" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="B152" t="s">
-        <v>76</v>
+        <v>143</v>
       </c>
       <c r="C152">
-        <v>43.38</v>
+        <v>102.34</v>
+      </c>
+      <c r="G152" t="s">
+        <v>174</v>
       </c>
     </row>
     <row r="153" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>175</v>
+        <v>244</v>
       </c>
       <c r="B153" t="s">
-        <v>145</v>
+        <v>123</v>
       </c>
       <c r="C153">
-        <v>102.34</v>
-      </c>
-      <c r="G153" t="s">
-        <v>176</v>
+        <v>213.3</v>
       </c>
     </row>
     <row r="154" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>246</v>
+        <v>198</v>
       </c>
       <c r="B154" t="s">
-        <v>123</v>
+        <v>150</v>
       </c>
       <c r="C154">
-        <v>213.3</v>
+        <v>246.07</v>
       </c>
     </row>
     <row r="155" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>200</v>
+        <v>257</v>
       </c>
       <c r="B155" t="s">
-        <v>152</v>
+        <v>69</v>
       </c>
       <c r="C155">
-        <v>246.07</v>
+        <v>173.97</v>
       </c>
     </row>
     <row r="156" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>259</v>
+        <v>186</v>
       </c>
       <c r="B156" t="s">
-        <v>69</v>
+        <v>169</v>
       </c>
       <c r="C156">
-        <v>173.97</v>
+        <v>119.78</v>
       </c>
     </row>
     <row r="157" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>188</v>
+        <v>336</v>
       </c>
       <c r="B157" t="s">
-        <v>171</v>
+        <v>337</v>
       </c>
       <c r="C157">
-        <v>119.78</v>
+        <v>119.14</v>
+      </c>
+      <c r="D157">
+        <f>4.2*23</f>
+        <v>96.600000000000009</v>
+      </c>
+      <c r="E157">
+        <f>4.2*23</f>
+        <v>96.600000000000009</v>
+      </c>
+      <c r="F157">
+        <v>0</v>
+      </c>
+      <c r="G157" t="s">
+        <v>341</v>
+      </c>
+      <c r="I157" s="2">
+        <v>0.5</v>
       </c>
     </row>
     <row r="158" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>338</v>
+        <v>3</v>
       </c>
       <c r="B158" t="s">
-        <v>339</v>
+        <v>4</v>
       </c>
       <c r="C158">
-        <v>119.14</v>
-      </c>
-      <c r="D158">
-        <f>4.2*23</f>
-        <v>96.600000000000009</v>
-      </c>
-      <c r="E158">
-        <f>4.2*23</f>
-        <v>96.600000000000009</v>
-      </c>
-      <c r="F158">
-        <v>0</v>
-      </c>
-      <c r="G158" t="s">
-        <v>343</v>
-      </c>
-      <c r="I158" s="2">
-        <v>0.5</v>
+        <v>115.37</v>
       </c>
     </row>
     <row r="159" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>3</v>
+        <v>302</v>
       </c>
       <c r="B159" t="s">
-        <v>4</v>
+        <v>295</v>
       </c>
       <c r="C159">
-        <v>115.37</v>
-      </c>
-    </row>
-    <row r="160" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A160" t="s">
-        <v>304</v>
-      </c>
-      <c r="B160" t="s">
-        <v>297</v>
-      </c>
-      <c r="C160">
         <v>30.51</v>
       </c>
-      <c r="D160">
+      <c r="D159">
         <f>3.8*12</f>
         <v>45.599999999999994</v>
       </c>
-      <c r="E160">
+      <c r="E159">
         <f>3.8*12</f>
         <v>45.599999999999994</v>
       </c>
-      <c r="F160">
+      <c r="F159">
         <v>0</v>
       </c>
-      <c r="G160" t="s">
-        <v>347</v>
-      </c>
-      <c r="I160" s="2">
+      <c r="G159" t="s">
+        <v>345</v>
+      </c>
+      <c r="I159" s="2">
         <v>0.6</v>
+      </c>
+    </row>
+    <row r="160" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A160" s="3" t="s">
+        <v>338</v>
+      </c>
+      <c r="B160" s="3" t="s">
+        <v>339</v>
+      </c>
+      <c r="C160" s="3">
+        <v>37.25</v>
+      </c>
+      <c r="D160" s="3">
+        <f>1.95*20</f>
+        <v>39</v>
+      </c>
+      <c r="E160" s="3">
+        <f>1.95*20</f>
+        <v>39</v>
+      </c>
+      <c r="F160" s="3">
+        <v>0</v>
+      </c>
+      <c r="G160" s="3" t="s">
+        <v>340</v>
+      </c>
+      <c r="H160" s="4"/>
+      <c r="I160" s="4">
+        <v>0.5</v>
       </c>
     </row>
     <row r="161" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A161" s="3" t="s">
-        <v>340</v>
+        <v>60</v>
       </c>
       <c r="B161" s="3" t="s">
-        <v>341</v>
+        <v>61</v>
       </c>
       <c r="C161" s="3">
         <v>37.25</v>
       </c>
-      <c r="D161" s="3">
-        <f>1.95*20</f>
-        <v>39</v>
-      </c>
-      <c r="E161" s="3">
-        <f>1.95*20</f>
-        <v>39</v>
-      </c>
-      <c r="F161" s="3">
-        <v>0</v>
-      </c>
-      <c r="G161" s="3" t="s">
-        <v>342</v>
-      </c>
       <c r="H161" s="4"/>
-      <c r="I161" s="4">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="162" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A162" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="B162" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="C162" s="3">
-        <v>37.25</v>
-      </c>
-      <c r="H162" s="4"/>
-      <c r="I162" s="4"/>
-    </row>
-    <row r="163" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="I161" s="4"/>
+    </row>
+    <row r="162" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A162" t="s">
+        <v>99</v>
+      </c>
+      <c r="B162" t="s">
+        <v>100</v>
+      </c>
+      <c r="C162">
+        <v>21.9</v>
+      </c>
+    </row>
+    <row r="163" spans="1:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>99</v>
+        <v>216</v>
       </c>
       <c r="B163" t="s">
-        <v>100</v>
+        <v>146</v>
       </c>
       <c r="C163">
-        <v>21.9</v>
-      </c>
-    </row>
-    <row r="164" spans="1:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A164" t="s">
-        <v>218</v>
-      </c>
-      <c r="B164" t="s">
-        <v>148</v>
-      </c>
-      <c r="C164">
         <v>47.58</v>
       </c>
-      <c r="D164">
+      <c r="D163">
         <f>4.3*(15+1)</f>
         <v>68.8</v>
       </c>
-      <c r="E164">
+      <c r="E163">
         <f>4.3*(15+1)</f>
         <v>68.8</v>
       </c>
-      <c r="F164">
+      <c r="F163">
         <v>0</v>
       </c>
-      <c r="G164" t="s">
-        <v>351</v>
-      </c>
-      <c r="I164" s="2">
+      <c r="G163" t="s">
+        <v>349</v>
+      </c>
+      <c r="I163" s="2">
         <v>0.45</v>
       </c>
     </row>
-    <row r="165" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A164" t="s">
+        <v>217</v>
+      </c>
+      <c r="B164" t="s">
+        <v>159</v>
+      </c>
+      <c r="C164">
+        <v>64.11</v>
+      </c>
+    </row>
+    <row r="165" spans="1:14" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>219</v>
+        <v>183</v>
       </c>
       <c r="B165" t="s">
-        <v>161</v>
+        <v>141</v>
       </c>
       <c r="C165">
-        <v>64.11</v>
-      </c>
-    </row>
-    <row r="166" spans="1:14" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A166" t="s">
-        <v>185</v>
-      </c>
-      <c r="B166" t="s">
-        <v>143</v>
-      </c>
-      <c r="C166">
         <v>126.63</v>
       </c>
     </row>
-    <row r="167" spans="1:14" s="3" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A167" s="3" t="s">
-        <v>280</v>
-      </c>
-      <c r="B167" s="3" t="s">
-        <v>281</v>
-      </c>
-      <c r="C167" s="3">
+    <row r="166" spans="1:14" s="3" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A166" s="3" t="s">
+        <v>278</v>
+      </c>
+      <c r="B166" s="3" t="s">
+        <v>279</v>
+      </c>
+      <c r="C166" s="3">
         <v>89.63</v>
       </c>
-      <c r="D167" s="3">
+      <c r="D166" s="3">
         <f>12.62*10</f>
         <v>126.19999999999999</v>
       </c>
-      <c r="E167" s="3">
+      <c r="E166" s="3">
         <f>12.62*10</f>
         <v>126.19999999999999</v>
       </c>
-      <c r="F167" s="3">
+      <c r="F166" s="3">
         <v>0</v>
       </c>
-      <c r="G167" s="3" t="s">
-        <v>355</v>
-      </c>
-      <c r="H167" s="4"/>
-      <c r="I167" s="4">
+      <c r="G166" s="3" t="s">
+        <v>353</v>
+      </c>
+      <c r="H166" s="4"/>
+      <c r="I166" s="4">
         <v>0.65</v>
+      </c>
+    </row>
+    <row r="167" spans="1:14" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A167" t="s">
+        <v>218</v>
+      </c>
+      <c r="B167" t="s">
+        <v>219</v>
+      </c>
+      <c r="C167">
+        <v>16.88</v>
+      </c>
+      <c r="D167">
+        <f>E167/(1+I167)</f>
+        <v>12.096774193548386</v>
+      </c>
+      <c r="E167">
+        <f>225*20/248</f>
+        <v>18.14516129032258</v>
+      </c>
+      <c r="F167">
+        <v>0</v>
+      </c>
+      <c r="G167" t="s">
+        <v>406</v>
+      </c>
+      <c r="I167" s="2">
+        <v>0.5</v>
       </c>
     </row>
     <row r="168" spans="1:14" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>220</v>
+        <v>311</v>
       </c>
       <c r="B168" t="s">
-        <v>221</v>
+        <v>308</v>
       </c>
       <c r="C168">
-        <v>16.88</v>
-      </c>
-      <c r="D168">
-        <f>E168/(1+I168)</f>
-        <v>12.096774193548386</v>
-      </c>
-      <c r="E168">
-        <f>225*20/248</f>
-        <v>18.14516129032258</v>
-      </c>
-      <c r="F168">
-        <v>0</v>
+        <v>80.12</v>
       </c>
       <c r="G168" t="s">
-        <v>408</v>
-      </c>
-      <c r="I168" s="2">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="169" spans="1:14" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="169" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>313</v>
+        <v>110</v>
       </c>
       <c r="B169" t="s">
-        <v>310</v>
+        <v>111</v>
       </c>
       <c r="C169">
-        <v>80.12</v>
-      </c>
-      <c r="G169" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="170" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A170" t="s">
-        <v>110</v>
-      </c>
-      <c r="B170" t="s">
-        <v>111</v>
-      </c>
-      <c r="C170">
         <v>43.7</v>
       </c>
     </row>
-    <row r="171" spans="1:14" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A171" s="3" t="s">
-        <v>266</v>
-      </c>
-      <c r="B171" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="C171" s="3">
+    <row r="170" spans="1:14" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A170" s="3" t="s">
+        <v>264</v>
+      </c>
+      <c r="B170" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="C170" s="3">
         <v>35.01</v>
       </c>
-      <c r="D171" s="3">
+      <c r="D170" s="3">
         <f>700/332+600*20/332+1000/332</f>
         <v>41.265060240963855</v>
       </c>
-      <c r="E171" s="3">
+      <c r="E170" s="3">
         <f>700/332+600*20/332+1000/332</f>
         <v>41.265060240963855</v>
       </c>
-      <c r="F171" s="3">
+      <c r="F170" s="3">
         <f>700/332</f>
         <v>2.1084337349397591</v>
       </c>
-      <c r="G171" s="3" t="s">
-        <v>393</v>
-      </c>
-      <c r="H171" s="4"/>
-      <c r="I171" s="4">
+      <c r="G170" s="3" t="s">
+        <v>391</v>
+      </c>
+      <c r="H170" s="4"/>
+      <c r="I170" s="4">
         <v>0.65</v>
+      </c>
+    </row>
+    <row r="171" spans="1:14" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A171" t="s">
+        <v>31</v>
+      </c>
+      <c r="B171" t="s">
+        <v>31</v>
+      </c>
+      <c r="C171">
+        <v>85.44</v>
       </c>
     </row>
     <row r="172" spans="1:14" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>31</v>
+        <v>135</v>
       </c>
       <c r="B172" t="s">
-        <v>31</v>
+        <v>135</v>
       </c>
       <c r="C172">
-        <v>85.44</v>
-      </c>
-    </row>
-    <row r="173" spans="1:14" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+        <v>98.37</v>
+      </c>
+    </row>
+    <row r="173" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>137</v>
+        <v>208</v>
       </c>
       <c r="B173" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="C173">
-        <v>98.37</v>
-      </c>
-    </row>
-    <row r="174" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A174" t="s">
-        <v>210</v>
-      </c>
-      <c r="B174" t="s">
-        <v>134</v>
-      </c>
-      <c r="C174">
         <v>53.21</v>
       </c>
     </row>
-    <row r="175" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A175" s="5" t="s">
-        <v>406</v>
-      </c>
-      <c r="B175" s="5" t="s">
-        <v>405</v>
-      </c>
-      <c r="C175" s="6">
+    <row r="174" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A174" s="5" t="s">
+        <v>404</v>
+      </c>
+      <c r="B174" s="5" t="s">
+        <v>403</v>
+      </c>
+      <c r="C174" s="6">
         <v>9.6</v>
       </c>
-      <c r="D175" s="6">
-        <f>E175/(1+I175)+F175</f>
+      <c r="D174" s="6">
+        <f>E174/(1+I174)+F174</f>
         <v>6.428571428571427</v>
       </c>
-      <c r="E175" s="6">
+      <c r="E174" s="6">
         <f>(450*8)/140</f>
         <v>25.714285714285715</v>
       </c>
-      <c r="F175" s="6">
+      <c r="F174" s="6">
         <f>(-450*3)/140</f>
         <v>-9.6428571428571423</v>
       </c>
-      <c r="G175" s="5" t="s">
+      <c r="G174" s="5" t="s">
+        <v>405</v>
+      </c>
+      <c r="I174" s="7">
+        <v>0.6</v>
+      </c>
+      <c r="J174" s="8"/>
+      <c r="K174" s="8"/>
+      <c r="L174" s="6" t="s">
+        <v>403</v>
+      </c>
+      <c r="M174" s="6">
+        <v>9.6</v>
+      </c>
+      <c r="N174" s="8" t="str">
+        <f t="shared" ref="N174" si="0">IF(B174=L174,"true","false")</f>
+        <v>true</v>
+      </c>
+    </row>
+    <row r="175" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A175" t="s">
         <v>407</v>
       </c>
-      <c r="I175" s="7">
+      <c r="B175" t="s">
+        <v>408</v>
+      </c>
+      <c r="D175">
+        <f>E175/(1+I175)+F175</f>
+        <v>53.114406779661017</v>
+      </c>
+      <c r="E175">
+        <f>2.2*30</f>
+        <v>66</v>
+      </c>
+      <c r="F175">
+        <f>1400/118</f>
+        <v>11.864406779661017</v>
+      </c>
+      <c r="G175" t="s">
+        <v>409</v>
+      </c>
+      <c r="I175" s="2">
         <v>0.6</v>
       </c>
-      <c r="J175" s="8"/>
-      <c r="K175" s="8"/>
-      <c r="L175" s="6" t="s">
-        <v>405</v>
-      </c>
-      <c r="M175" s="6">
-        <v>9.6</v>
-      </c>
-      <c r="N175" s="8" t="str">
-        <f t="shared" ref="N175" si="0">IF(B175=L175,"true","false")</f>
-        <v>true</v>
-      </c>
+      <c r="J175" s="1"/>
     </row>
     <row r="176" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>409</v>
+        <v>411</v>
       </c>
       <c r="B176" t="s">
-        <v>410</v>
+        <v>412</v>
       </c>
       <c r="D176">
         <f>E176/(1+I176)+F176</f>
-        <v>53.114406779661017</v>
+        <v>32.234999999999999</v>
       </c>
       <c r="E176">
-        <f>2.2*30</f>
-        <v>66</v>
+        <f>700*7/100</f>
+        <v>49</v>
       </c>
       <c r="F176">
-        <f>1400/118</f>
-        <v>11.864406779661017</v>
+        <f>161/100</f>
+        <v>1.61</v>
       </c>
       <c r="G176" t="s">
-        <v>411</v>
+        <v>413</v>
       </c>
       <c r="I176" s="2">
         <v>0.6</v>
       </c>
       <c r="J176" s="1"/>
     </row>
-    <row r="177" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A177" t="s">
+        <v>416</v>
+      </c>
+      <c r="B177" t="s">
+        <v>417</v>
+      </c>
+      <c r="D177">
+        <f>E177/(1+I177)+F177</f>
+        <v>15.94896331738437</v>
+      </c>
+      <c r="E177">
+        <f>50*100/190</f>
+        <v>26.315789473684209</v>
+      </c>
+      <c r="F177">
+        <v>0</v>
+      </c>
+      <c r="G177" t="s">
+        <v>418</v>
+      </c>
+      <c r="I177" s="2">
+        <v>0.65</v>
+      </c>
       <c r="J177" s="1"/>
     </row>
-    <row r="178" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A178" t="s">
+        <v>419</v>
+      </c>
+      <c r="B178" t="s">
+        <v>420</v>
+      </c>
+      <c r="D178">
+        <f>(E178/(1+I178)+F178)</f>
+        <v>23.433333333333334</v>
+      </c>
+      <c r="E178">
+        <f>1.9*18.5</f>
+        <v>35.15</v>
+      </c>
+      <c r="F178">
+        <v>0</v>
+      </c>
+      <c r="G178" t="s">
+        <v>421</v>
+      </c>
+      <c r="I178" s="2">
+        <v>0.5</v>
+      </c>
       <c r="J178" s="1"/>
     </row>
-    <row r="179" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:10" x14ac:dyDescent="0.25">
       <c r="J179" s="1"/>
     </row>
-    <row r="180" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:10" x14ac:dyDescent="0.25">
       <c r="J180" s="1"/>
     </row>
-    <row r="181" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:10" x14ac:dyDescent="0.25">
       <c r="J181" s="1"/>
     </row>
-    <row r="182" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:10" x14ac:dyDescent="0.25">
       <c r="J182" s="1"/>
     </row>
-    <row r="183" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:10" x14ac:dyDescent="0.25">
       <c r="J183" s="1"/>
     </row>
-    <row r="184" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:10" x14ac:dyDescent="0.25">
       <c r="J184" s="1"/>
     </row>
-    <row r="185" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:10" x14ac:dyDescent="0.25">
       <c r="J185" s="1"/>
     </row>
-    <row r="186" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:10" x14ac:dyDescent="0.25">
       <c r="J186" s="1"/>
     </row>
-    <row r="187" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:10" x14ac:dyDescent="0.25">
       <c r="J187" s="1"/>
     </row>
-    <row r="188" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:10" x14ac:dyDescent="0.25">
       <c r="J188" s="1"/>
     </row>
-    <row r="189" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:10" x14ac:dyDescent="0.25">
       <c r="J189" s="1"/>
     </row>
-    <row r="190" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:10" x14ac:dyDescent="0.25">
       <c r="J190" s="1"/>
     </row>
-    <row r="191" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:10" x14ac:dyDescent="0.25">
       <c r="J191" s="1"/>
     </row>
-    <row r="192" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:10" x14ac:dyDescent="0.25">
       <c r="J192" s="1"/>
     </row>
     <row r="193" spans="10:10" x14ac:dyDescent="0.25">
@@ -5667,9 +5808,6 @@
     </row>
     <row r="500" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J500" s="1"/>
-    </row>
-    <row r="501" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J501" s="1"/>
     </row>
   </sheetData>
   <sortState ref="A3:P183">
@@ -5682,20 +5820,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F24"/>
+  <dimension ref="A1:F26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="F1" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -5703,23 +5841,23 @@
         <v>30</v>
       </c>
       <c r="F2" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F3" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F4" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -5727,12 +5865,12 @@
         <v>24</v>
       </c>
       <c r="F5" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -5742,17 +5880,17 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -5762,32 +5900,32 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
@@ -5797,12 +5935,12 @@
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
@@ -5817,12 +5955,22 @@
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>11</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>114</v>
       </c>
     </row>
   </sheetData>

</xml_diff>